<commit_message>
TFL Performance Test Reports updated
</commit_message>
<xml_diff>
--- a/TFL_PlanMyJourney_TestReport.xlsx
+++ b/TFL_PlanMyJourney_TestReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6127e3540350f1f4/Desktop/TFL_Performancetesting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6127e3540350f1f4/Desktop/TFL_Performancetesting/PerformanceTestTFL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="14_{8E2B4AF1-645E-484F-86A2-7808C4A3F3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9CE3AE5-1B1D-453E-8EE1-A7B3062CF6AC}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="14_{8E2B4AF1-645E-484F-86A2-7808C4A3F3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03EDFBBC-AC21-4EB0-B60A-2B25F137F079}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Label</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t xml:space="preserve">500/Internal Server Error	</t>
-  </si>
-  <si>
-    <t>Encountered 500 server response from PlanMyJourney for future time</t>
   </si>
   <si>
     <t>TFL02_T02_launch1/-158</t>
@@ -226,12 +223,18 @@
 3. TFL02_T03_ToStopDetails 
 4. TFL02_T04_PlanMyJourney</t>
   </si>
+  <si>
+    <t>https://tfl.gov.uk/JourneyPlanner/ResultsAsync?InputFrom=Kensington+%28Olympia%29&amp;FromId=1000170&amp;InputTo=Amersham&amp;ToId=1000006&amp;Date=20230506&amp;Time=0045&amp;app_id=8268063a&amp;app_key=14f7f5ff5d64df2e88701cef2049c804</t>
+  </si>
+  <si>
+    <t>The server responded with a 500 error code when attempting to use the PlanMyJourney functionality for future time.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +284,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -447,12 +458,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -514,6 +526,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -533,9 +551,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -544,12 +559,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -985,10 +1001,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1326,18 +1338,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
@@ -1358,10 +1370,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>22</v>
@@ -1372,56 +1384,56 @@
         <v>24</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
+      <c r="A7" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="37">
+        <v>40</v>
+      </c>
+      <c r="B10" s="27">
         <v>44990.603472222225</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="26">
         <v>44990.624305555553</v>
@@ -1431,7 +1443,7 @@
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="11">
         <v>50</v>
@@ -1480,20 +1492,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1534,8 +1546,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
-        <v>48</v>
+      <c r="A3" s="35" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>30</v>
@@ -1572,7 +1584,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="15" t="s">
         <v>31</v>
       </c>
@@ -1608,7 +1620,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="15" t="s">
         <v>32</v>
       </c>
@@ -1644,11 +1656,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
-        <v>47</v>
+      <c r="A6" s="36" t="s">
+        <v>46</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="21">
         <v>325</v>
@@ -1682,7 +1694,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="35"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="20" t="s">
         <v>27</v>
       </c>
@@ -1718,7 +1730,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="20" t="s">
         <v>28</v>
       </c>
@@ -1754,7 +1766,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="35"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="20" t="s">
         <v>29</v>
       </c>
@@ -1814,15 +1826,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.26953125" style="8" customWidth="1"/>
     <col min="2" max="2" width="54.54296875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.90625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="8" customWidth="1"/>
     <col min="5" max="5" width="61.1796875" style="8" customWidth="1"/>
     <col min="6" max="16384" width="9.1796875" style="8"/>
@@ -1845,19 +1857,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="23">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>29</v>
+      <c r="C2" s="38" t="s">
+        <v>52</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="11" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>